<commit_message>
fixed pie charts and updated data
</commit_message>
<xml_diff>
--- a/data/Sell_Ygo!.xlsx
+++ b/data/Sell_Ygo!.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leftis\OneDrive - City, University of London\Desktop\elef\Ygo!\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DE255E-1B5B-4F91-8EC3-5F8E5E5C2112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD3955B-B6AA-4189-80E6-F519948C5DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="For Sale-Trade" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="286">
   <si>
     <t>Name</t>
   </si>
@@ -774,15 +774,9 @@
     <t>LD10</t>
   </si>
   <si>
-    <t>Decode Talker</t>
-  </si>
-  <si>
     <t>Quarter Century Secret Rare</t>
   </si>
   <si>
-    <t>TN23</t>
-  </si>
-  <si>
     <t>Dinomorphia Domain</t>
   </si>
   <si>
@@ -834,40 +828,73 @@
     <t>Performapal Odd-Eyes Seer</t>
   </si>
   <si>
+    <t>Tales of the White Forest</t>
+  </si>
+  <si>
+    <t>Blackwing - Shamal the Sandstorm</t>
+  </si>
+  <si>
+    <t>My Friend Purrely</t>
+  </si>
+  <si>
+    <t>RA02</t>
+  </si>
+  <si>
+    <t>Floowandereeze and the Advent of Adventure</t>
+  </si>
+  <si>
+    <t>Maple Maiden</t>
+  </si>
+  <si>
+    <t>Simorgh, Bird of Perfection</t>
+  </si>
+  <si>
+    <t>Super-Nimble Mega Hamster</t>
+  </si>
+  <si>
+    <t>Shamisen Samsara Sorrowcat</t>
+  </si>
+  <si>
+    <t>Dinomorphia Therizia</t>
+  </si>
+  <si>
+    <t>R-Genex Turing</t>
+  </si>
+  <si>
+    <t>BLTR</t>
+  </si>
+  <si>
+    <t>Infernoid Patrulea</t>
+  </si>
+  <si>
+    <t>Substitoad</t>
+  </si>
+  <si>
+    <t>Maximum Six</t>
+  </si>
+  <si>
+    <t>LODT</t>
+  </si>
+  <si>
+    <t>2024 Reprint</t>
+  </si>
+  <si>
+    <t>Gold Pride - Eradicator</t>
+  </si>
+  <si>
+    <t>LEDE</t>
+  </si>
+  <si>
     <t>Silhouhatte Rabbit</t>
   </si>
   <si>
+    <t>Illusion</t>
+  </si>
+  <si>
     <t>Mimighoul Dungeon</t>
   </si>
   <si>
-    <t>Tales of the White Forest</t>
-  </si>
-  <si>
-    <t>Blackwing - Shamal the Sandstorm</t>
-  </si>
-  <si>
-    <t>My Friend Purrely</t>
-  </si>
-  <si>
-    <t>RA02</t>
-  </si>
-  <si>
-    <t>Floowandereeze and the Advent of Adventure</t>
-  </si>
-  <si>
-    <t>Maple Maiden</t>
-  </si>
-  <si>
-    <t>Simorgh, Bird of Perfection</t>
-  </si>
-  <si>
-    <t>Super-Nimble Mega Hamster</t>
-  </si>
-  <si>
-    <t>Shamisen Samsara Sorrowcat</t>
-  </si>
-  <si>
-    <t>Dinomorphia Therizia</t>
+    <t>Mimighoul Maker</t>
   </si>
 </sst>
 </file>
@@ -1199,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q159"/>
+  <dimension ref="A1:Q164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5598,54 +5625,48 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B138" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C138" t="s">
-        <v>62</v>
+        <v>210</v>
       </c>
       <c r="D138" t="s">
-        <v>36</v>
-      </c>
-      <c r="E138">
-        <v>2300</v>
+        <v>43</v>
       </c>
       <c r="G138" t="s">
-        <v>246</v>
+        <v>21</v>
       </c>
       <c r="H138">
         <v>1</v>
       </c>
-      <c r="I138">
-        <v>3</v>
-      </c>
       <c r="L138" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="O138">
-        <v>0.51</v>
+        <v>0.3</v>
       </c>
       <c r="P138" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>247</v>
+      </c>
+      <c r="B139" t="s">
+        <v>27</v>
+      </c>
+      <c r="C139" t="s">
         <v>248</v>
       </c>
-      <c r="B139" t="s">
-        <v>42</v>
-      </c>
-      <c r="C139" t="s">
-        <v>210</v>
-      </c>
       <c r="D139" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G139" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="H139">
         <v>1</v>
@@ -5654,7 +5675,7 @@
         <v>237</v>
       </c>
       <c r="O139">
-        <v>0.3</v>
+        <v>6.69</v>
       </c>
       <c r="P139" t="s">
         <v>89</v>
@@ -5665,25 +5686,34 @@
         <v>249</v>
       </c>
       <c r="B140" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="C140" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="D140" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="E140">
+        <v>1400</v>
+      </c>
+      <c r="F140">
+        <v>2500</v>
       </c>
       <c r="G140" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="H140">
         <v>1</v>
+      </c>
+      <c r="J140">
+        <v>7</v>
       </c>
       <c r="L140" t="s">
         <v>237</v>
       </c>
       <c r="O140">
-        <v>6.69</v>
+        <v>0.1</v>
       </c>
       <c r="P140" t="s">
         <v>89</v>
@@ -5691,37 +5721,28 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B141" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C141" t="s">
-        <v>49</v>
+        <v>248</v>
       </c>
       <c r="D141" t="s">
-        <v>20</v>
-      </c>
-      <c r="E141">
-        <v>1400</v>
-      </c>
-      <c r="F141">
-        <v>2500</v>
+        <v>28</v>
       </c>
       <c r="G141" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="H141">
         <v>1</v>
-      </c>
-      <c r="J141">
-        <v>7</v>
       </c>
       <c r="L141" t="s">
         <v>237</v>
       </c>
       <c r="O141">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="P141" t="s">
         <v>89</v>
@@ -5729,19 +5750,19 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B142" t="s">
         <v>27</v>
       </c>
       <c r="C142" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D142" t="s">
         <v>28</v>
       </c>
       <c r="G142" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="H142">
         <v>1</v>
@@ -5750,7 +5771,7 @@
         <v>237</v>
       </c>
       <c r="O142">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="P142" t="s">
         <v>89</v>
@@ -5760,17 +5781,8 @@
       <c r="A143" t="s">
         <v>253</v>
       </c>
-      <c r="B143" t="s">
-        <v>27</v>
-      </c>
-      <c r="C143" t="s">
-        <v>254</v>
-      </c>
-      <c r="D143" t="s">
-        <v>28</v>
-      </c>
       <c r="G143" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="H143">
         <v>1</v>
@@ -5779,7 +5791,7 @@
         <v>237</v>
       </c>
       <c r="O143">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="P143" t="s">
         <v>89</v>
@@ -5787,10 +5799,10 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G144" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="H144">
         <v>1</v>
@@ -5807,10 +5819,10 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G145" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="H145">
         <v>1</v>
@@ -5819,7 +5831,7 @@
         <v>237</v>
       </c>
       <c r="O145">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="P145" t="s">
         <v>89</v>
@@ -5827,7 +5839,7 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G146" t="s">
         <v>37</v>
@@ -5836,10 +5848,10 @@
         <v>1</v>
       </c>
       <c r="L146" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="O146">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="P146" t="s">
         <v>89</v>
@@ -5847,19 +5859,40 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>258</v>
+        <v>262</v>
+      </c>
+      <c r="B147" t="s">
+        <v>57</v>
+      </c>
+      <c r="C147" t="s">
+        <v>19</v>
+      </c>
+      <c r="D147" t="s">
+        <v>108</v>
+      </c>
+      <c r="E147">
+        <v>100</v>
+      </c>
+      <c r="F147">
+        <v>1800</v>
       </c>
       <c r="G147" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="H147">
+        <v>2</v>
+      </c>
+      <c r="J147">
+        <v>6</v>
+      </c>
+      <c r="K147">
         <v>1</v>
       </c>
       <c r="L147" t="s">
-        <v>259</v>
+        <v>109</v>
       </c>
       <c r="O147">
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
       <c r="P147" t="s">
         <v>89</v>
@@ -5867,37 +5900,25 @@
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="B148" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="C148" t="s">
-        <v>19</v>
+        <v>210</v>
       </c>
       <c r="D148" t="s">
-        <v>108</v>
-      </c>
-      <c r="E148">
-        <v>100</v>
-      </c>
-      <c r="F148">
-        <v>1800</v>
+        <v>28</v>
       </c>
       <c r="G148" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="H148">
-        <v>2</v>
-      </c>
-      <c r="J148">
-        <v>6</v>
-      </c>
-      <c r="K148">
         <v>1</v>
       </c>
       <c r="L148" t="s">
-        <v>109</v>
+        <v>257</v>
       </c>
       <c r="P148" t="s">
         <v>89</v>
@@ -5905,19 +5926,19 @@
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G149" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="H149">
         <v>1</v>
       </c>
       <c r="L149" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="O149">
-        <v>11.85</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="P149" t="s">
         <v>89</v>
@@ -5925,19 +5946,19 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G150" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="H150">
         <v>1</v>
       </c>
       <c r="L150" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="O150">
-        <v>7.02</v>
+        <v>0.5</v>
       </c>
       <c r="P150" t="s">
         <v>89</v>
@@ -5945,19 +5966,19 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G151" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="H151">
         <v>1</v>
       </c>
       <c r="L151" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="O151">
-        <v>4.3099999999999996</v>
+        <v>1.05</v>
       </c>
       <c r="P151" t="s">
         <v>89</v>
@@ -5965,7 +5986,7 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G152" t="s">
         <v>118</v>
@@ -5977,7 +5998,7 @@
         <v>237</v>
       </c>
       <c r="O152">
-        <v>0.5</v>
+        <v>0.79</v>
       </c>
       <c r="P152" t="s">
         <v>89</v>
@@ -5985,19 +6006,19 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G153" t="s">
-        <v>118</v>
+        <v>21</v>
       </c>
       <c r="H153">
         <v>1</v>
       </c>
       <c r="L153" t="s">
-        <v>270</v>
+        <v>237</v>
       </c>
       <c r="O153">
-        <v>1.05</v>
+        <v>0.05</v>
       </c>
       <c r="P153" t="s">
         <v>89</v>
@@ -6005,10 +6026,10 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G154" t="s">
-        <v>118</v>
+        <v>21</v>
       </c>
       <c r="H154">
         <v>1</v>
@@ -6017,7 +6038,7 @@
         <v>237</v>
       </c>
       <c r="O154">
-        <v>0.79</v>
+        <v>0.25</v>
       </c>
       <c r="P154" t="s">
         <v>89</v>
@@ -6025,7 +6046,7 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G155" t="s">
         <v>21</v>
@@ -6034,10 +6055,10 @@
         <v>1</v>
       </c>
       <c r="L155" t="s">
-        <v>237</v>
+        <v>266</v>
       </c>
       <c r="O155">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="P155" t="s">
         <v>89</v>
@@ -6045,7 +6066,7 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G156" t="s">
         <v>21</v>
@@ -6057,7 +6078,7 @@
         <v>237</v>
       </c>
       <c r="O156">
-        <v>0.25</v>
+        <v>0.12</v>
       </c>
       <c r="P156" t="s">
         <v>89</v>
@@ -6065,19 +6086,19 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G157" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="H157">
         <v>1</v>
       </c>
       <c r="L157" t="s">
-        <v>270</v>
+        <v>237</v>
       </c>
       <c r="O157">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="P157" t="s">
         <v>89</v>
@@ -6085,7 +6106,22 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>275</v>
+        <v>273</v>
+      </c>
+      <c r="B158" t="s">
+        <v>57</v>
+      </c>
+      <c r="C158" t="s">
+        <v>19</v>
+      </c>
+      <c r="D158" t="s">
+        <v>20</v>
+      </c>
+      <c r="E158">
+        <v>600</v>
+      </c>
+      <c r="F158">
+        <v>600</v>
       </c>
       <c r="G158" t="s">
         <v>21</v>
@@ -6093,11 +6129,17 @@
       <c r="H158">
         <v>1</v>
       </c>
+      <c r="J158">
+        <v>2</v>
+      </c>
       <c r="L158" t="s">
-        <v>237</v>
+        <v>274</v>
+      </c>
+      <c r="N158" t="s">
+        <v>58</v>
       </c>
       <c r="O158">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="P158" t="s">
         <v>89</v>
@@ -6105,21 +6147,220 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>275</v>
+      </c>
+      <c r="B159" t="s">
+        <v>48</v>
+      </c>
+      <c r="C159" t="s">
+        <v>45</v>
+      </c>
+      <c r="D159" t="s">
+        <v>20</v>
+      </c>
+      <c r="E159">
+        <v>1800</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="G159" t="s">
+        <v>21</v>
+      </c>
+      <c r="H159">
+        <v>1</v>
+      </c>
+      <c r="J159">
+        <v>4</v>
+      </c>
+      <c r="L159" t="s">
+        <v>274</v>
+      </c>
+      <c r="O159">
+        <v>0.08</v>
+      </c>
+      <c r="P159" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>276</v>
       </c>
-      <c r="G159" t="s">
-        <v>118</v>
-      </c>
-      <c r="H159">
-        <v>1</v>
-      </c>
-      <c r="L159" t="s">
-        <v>237</v>
-      </c>
-      <c r="O159">
-        <v>0.4</v>
-      </c>
-      <c r="P159" t="s">
+      <c r="B160" t="s">
+        <v>75</v>
+      </c>
+      <c r="C160" t="s">
+        <v>49</v>
+      </c>
+      <c r="D160" t="s">
+        <v>20</v>
+      </c>
+      <c r="E160">
+        <v>100</v>
+      </c>
+      <c r="F160">
+        <v>2000</v>
+      </c>
+      <c r="G160" t="s">
+        <v>103</v>
+      </c>
+      <c r="H160">
+        <v>1</v>
+      </c>
+      <c r="J160">
+        <v>1</v>
+      </c>
+      <c r="L160" t="s">
+        <v>274</v>
+      </c>
+      <c r="O160">
+        <v>4.3</v>
+      </c>
+      <c r="P160" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>277</v>
+      </c>
+      <c r="B161" t="s">
+        <v>24</v>
+      </c>
+      <c r="C161" t="s">
+        <v>60</v>
+      </c>
+      <c r="D161" t="s">
+        <v>20</v>
+      </c>
+      <c r="E161">
+        <v>1900</v>
+      </c>
+      <c r="F161">
+        <v>1600</v>
+      </c>
+      <c r="G161" t="s">
+        <v>21</v>
+      </c>
+      <c r="H161">
+        <v>1</v>
+      </c>
+      <c r="J161">
+        <v>6</v>
+      </c>
+      <c r="L161" t="s">
+        <v>278</v>
+      </c>
+      <c r="M161" t="s">
+        <v>279</v>
+      </c>
+      <c r="O161">
+        <v>1.6</v>
+      </c>
+      <c r="P161" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>280</v>
+      </c>
+      <c r="B162" t="s">
+        <v>57</v>
+      </c>
+      <c r="C162" t="s">
+        <v>60</v>
+      </c>
+      <c r="D162" t="s">
+        <v>71</v>
+      </c>
+      <c r="E162">
+        <v>2700</v>
+      </c>
+      <c r="F162">
+        <v>1700</v>
+      </c>
+      <c r="G162" t="s">
+        <v>245</v>
+      </c>
+      <c r="H162">
+        <v>1</v>
+      </c>
+      <c r="J162">
+        <v>8</v>
+      </c>
+      <c r="L162" t="s">
+        <v>281</v>
+      </c>
+      <c r="O162">
+        <v>4.3</v>
+      </c>
+      <c r="P162" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>282</v>
+      </c>
+      <c r="B163" t="s">
+        <v>18</v>
+      </c>
+      <c r="C163" t="s">
+        <v>283</v>
+      </c>
+      <c r="D163" t="s">
+        <v>36</v>
+      </c>
+      <c r="E163">
+        <v>1500</v>
+      </c>
+      <c r="G163" t="s">
+        <v>103</v>
+      </c>
+      <c r="H163">
+        <v>1</v>
+      </c>
+      <c r="I163">
+        <v>2</v>
+      </c>
+      <c r="L163" t="s">
+        <v>257</v>
+      </c>
+      <c r="O163">
+        <v>11.85</v>
+      </c>
+      <c r="P163" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>284</v>
+      </c>
+      <c r="B164" t="s">
+        <v>27</v>
+      </c>
+      <c r="C164" t="s">
+        <v>45</v>
+      </c>
+      <c r="D164" t="s">
+        <v>28</v>
+      </c>
+      <c r="G164" t="s">
+        <v>21</v>
+      </c>
+      <c r="H164">
+        <v>1</v>
+      </c>
+      <c r="L164" t="s">
+        <v>257</v>
+      </c>
+      <c r="O164">
+        <v>7.02</v>
+      </c>
+      <c r="P164" t="s">
         <v>89</v>
       </c>
     </row>
@@ -6154,19 +6395,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>

</xml_diff>